<commit_message>
update version finale tracking
</commit_message>
<xml_diff>
--- a/Traking/Winners_Tracking.xlsx
+++ b/Traking/Winners_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fef60bdfbb7e8819/Documents/GitHub/scrabble-td3-winners/Traking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{BDF0F77A-3A2C-42DE-B9C8-C8A399E87190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B7F53CA-F63F-4663-9F93-09BE88D861F0}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{BDF0F77A-3A2C-42DE-B9C8-C8A399E87190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CBD7576-334D-4789-A0A1-7F6E2F4C24F6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{69E16E0F-F538-B845-8F7F-630A124B2F74}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1012,7 +1012,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0FBA1522-4A75-4061-8A5F-F37A65DDD888}" name="Tableau croisé dynamique1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0FBA1522-4A75-4061-8A5F-F37A65DDD888}" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -1449,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAE7E2C-8C99-9742-8F88-0BE23F9A2024}">
   <dimension ref="B1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2224,7 +2224,7 @@
         <v>119</v>
       </c>
       <c r="D52" s="10">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.35">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D53" s="10">
         <f>H48-D52</f>
-        <v>-6.2000000000000011</v>
+        <v>5.7999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>